<commit_message>
Fix table, add new operators
</commit_message>
<xml_diff>
--- a/docs/PrecedenceTable.xlsx
+++ b/docs/PrecedenceTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\IFJ\KompIFJlator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52F9455-8A5B-4CC9-AD60-D4210E524B30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DDD305-4092-44E9-9664-A9916022F07C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{781F262C-900B-4A41-AA3A-3D1F6B84603C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{781F262C-900B-4A41-AA3A-3D1F6B84603C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="42">
   <si>
     <t>(</t>
   </si>
@@ -142,6 +142,24 @@
   </si>
   <si>
     <t>RuleNEq</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>E-&gt;-(E)</t>
+  </si>
+  <si>
+    <t>E-&gt;--E</t>
+  </si>
+  <si>
+    <t>RuleBra</t>
+  </si>
+  <si>
+    <t>RuleNe2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> maybe</t>
   </si>
 </sst>
 </file>
@@ -345,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -385,6 +403,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -397,13 +423,194 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="24">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -601,17 +808,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E39554DB-F2E3-4E09-891E-6102DB8BCFEB}" name="Table2" displayName="Table2" ref="B3:I10" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E39554DB-F2E3-4E09-891E-6102DB8BCFEB}" name="Table2" displayName="Table2" ref="B3:I10" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="B3:I10" xr:uid="{30E74BC2-71C2-498F-9B29-4594470EC22F}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{75725AC1-01A2-4C32-AF27-5E859459CBB2}" name=" " dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{1CDABF8C-D97D-4628-8B79-6114651AD016}" name="+, -" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{0D239569-6E34-451B-BB51-FDCD8FBA0FE4}" name="*, /" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{D7E63E17-754D-47B0-9EDB-FB5A8E3D9BED}" name="(" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{77970DFC-59BD-4966-AA61-7D6C1DEDB481}" name=")" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{B2BF0C15-EF2B-43B1-AA62-B2B234B13B3D}" name="i" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{7C9301D4-F080-4B11-B168-6D051E3A8901}" name="&lt;, &lt;=, &gt;, =&gt;, ==, !=" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{7E9414A9-1A3A-4EB6-89D9-A329C078092F}" name="$" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{75725AC1-01A2-4C32-AF27-5E859459CBB2}" name=" " dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{1CDABF8C-D97D-4628-8B79-6114651AD016}" name="+, -" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{0D239569-6E34-451B-BB51-FDCD8FBA0FE4}" name="*, /" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{D7E63E17-754D-47B0-9EDB-FB5A8E3D9BED}" name="(" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{77970DFC-59BD-4966-AA61-7D6C1DEDB481}" name=")" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{B2BF0C15-EF2B-43B1-AA62-B2B234B13B3D}" name="i" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{7C9301D4-F080-4B11-B168-6D051E3A8901}" name="&lt;, &lt;=, &gt;, =&gt;, ==, !=" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{7E9414A9-1A3A-4EB6-89D9-A329C078092F}" name="$" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A320B432-ECE4-4BBD-83BC-271845AE0C7D}" name="Table22" displayName="Table22" ref="B15:I22" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="B15:I22" xr:uid="{482FB508-FA20-460E-9777-8B46DD2DCC7E}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{B5AE6229-5992-428D-B083-4B4DC0EF3AF4}" name=" " dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{2476DCEA-4548-4B54-AA68-8C4ECAB4D82E}" name="+, -" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{1AC0833A-D33C-48A9-A5FD-E53C886647E2}" name="*, /" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{C74CD310-58A7-4695-A22D-8509CFCB2A49}" name="(" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{03B55521-36CC-4560-854F-0207E65282CB}" name=")" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{1D82CE22-06FC-4E20-80A3-98617010C5FF}" name="i" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{4E004535-EED5-454A-A7D2-9383492DFAD3}" name="&lt;, &lt;=, &gt;, =&gt;, ==, !=" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{A6C20564-2A4C-4E85-A3CD-F925DC6793F0}" name="$" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -917,7 +1141,7 @@
   <dimension ref="B2:AD28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,10 +1152,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="20"/>
+      <c r="L2" s="24"/>
       <c r="R2" s="16"/>
       <c r="S2" s="16"/>
       <c r="T2" s="17"/>
@@ -961,8 +1185,8 @@
       <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="21"/>
-      <c r="L3" s="22"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="26"/>
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
       <c r="T3" s="17"/>
@@ -1231,7 +1455,7 @@
       <c r="L12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="21" t="s">
         <v>32</v>
       </c>
       <c r="N12" s="17"/>
@@ -1240,6 +1464,9 @@
       <c r="T12" s="17"/>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
       <c r="K13" s="10">
         <v>10</v>
       </c>
@@ -1261,7 +1488,7 @@
       <c r="L14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="24" t="s">
+      <c r="M14" s="22" t="s">
         <v>34</v>
       </c>
       <c r="R14" s="18"/>
@@ -1269,13 +1496,37 @@
       <c r="T14" s="17"/>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>3</v>
+      </c>
       <c r="K15" s="13">
         <v>12</v>
       </c>
       <c r="L15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="M15" s="24" t="s">
+      <c r="M15" s="22" t="s">
         <v>35</v>
       </c>
       <c r="R15" s="18"/>
@@ -1283,61 +1534,215 @@
       <c r="T15" s="17"/>
     </row>
     <row r="16" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="I16" s="17"/>
+      <c r="B16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="J16" s="17"/>
       <c r="K16" s="18"/>
       <c r="R16" s="17"/>
       <c r="S16" s="17"/>
       <c r="T16" s="17"/>
     </row>
-    <row r="17" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="I17" s="17"/>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="J17" s="17"/>
-      <c r="K17" s="18"/>
+      <c r="K17" s="18">
+        <v>13</v>
+      </c>
+      <c r="L17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" t="s">
+        <v>41</v>
+      </c>
       <c r="R17" s="17"/>
       <c r="S17" s="17"/>
       <c r="T17" s="17"/>
     </row>
-    <row r="18" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="7"/>
       <c r="J18" s="17"/>
-      <c r="K18" s="18"/>
-    </row>
-    <row r="19" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
+      <c r="K18" s="18">
+        <v>14</v>
+      </c>
+      <c r="L18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="J19" s="17"/>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="J20" s="17"/>
       <c r="K20" s="18"/>
     </row>
-    <row r="21" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-    </row>
-    <row r="22" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-    </row>
-    <row r="23" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
     </row>
-    <row r="25" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I25" s="17"/>
     </row>
-    <row r="28" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="J28" s="17"/>
     </row>
   </sheetData>
@@ -1347,8 +1752,9 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Awful code, but should be working
</commit_message>
<xml_diff>
--- a/docs/PrecedenceTable.xlsx
+++ b/docs/PrecedenceTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\IFJ\KompIFJlator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DDD305-4092-44E9-9664-A9916022F07C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D16AF8C-34DA-4D70-9961-BD74CBD3CCFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{781F262C-900B-4A41-AA3A-3D1F6B84603C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{781F262C-900B-4A41-AA3A-3D1F6B84603C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="38">
   <si>
     <t>(</t>
   </si>
@@ -147,19 +147,7 @@
     <t>v2</t>
   </si>
   <si>
-    <t>E-&gt;-(E)</t>
-  </si>
-  <si>
-    <t>E-&gt;--E</t>
-  </si>
-  <si>
-    <t>RuleBra</t>
-  </si>
-  <si>
-    <t>RuleNe2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> maybe</t>
+    <t>v2 Unary</t>
   </si>
 </sst>
 </file>
@@ -363,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -411,6 +399,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -427,7 +421,190 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="36">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -808,34 +985,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E39554DB-F2E3-4E09-891E-6102DB8BCFEB}" name="Table2" displayName="Table2" ref="B3:I10" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E39554DB-F2E3-4E09-891E-6102DB8BCFEB}" name="Table2" displayName="Table2" ref="B3:I10" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
   <autoFilter ref="B3:I10" xr:uid="{30E74BC2-71C2-498F-9B29-4594470EC22F}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{75725AC1-01A2-4C32-AF27-5E859459CBB2}" name=" " dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{1CDABF8C-D97D-4628-8B79-6114651AD016}" name="+, -" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{0D239569-6E34-451B-BB51-FDCD8FBA0FE4}" name="*, /" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{D7E63E17-754D-47B0-9EDB-FB5A8E3D9BED}" name="(" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{77970DFC-59BD-4966-AA61-7D6C1DEDB481}" name=")" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{B2BF0C15-EF2B-43B1-AA62-B2B234B13B3D}" name="i" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{7C9301D4-F080-4B11-B168-6D051E3A8901}" name="&lt;, &lt;=, &gt;, =&gt;, ==, !=" dataDxfId="13"/>
-    <tableColumn id="15" xr3:uid="{7E9414A9-1A3A-4EB6-89D9-A329C078092F}" name="$" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{75725AC1-01A2-4C32-AF27-5E859459CBB2}" name=" " dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{1CDABF8C-D97D-4628-8B79-6114651AD016}" name="+, -" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{0D239569-6E34-451B-BB51-FDCD8FBA0FE4}" name="*, /" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{D7E63E17-754D-47B0-9EDB-FB5A8E3D9BED}" name="(" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{77970DFC-59BD-4966-AA61-7D6C1DEDB481}" name=")" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{B2BF0C15-EF2B-43B1-AA62-B2B234B13B3D}" name="i" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{7C9301D4-F080-4B11-B168-6D051E3A8901}" name="&lt;, &lt;=, &gt;, =&gt;, ==, !=" dataDxfId="25"/>
+    <tableColumn id="15" xr3:uid="{7E9414A9-1A3A-4EB6-89D9-A329C078092F}" name="$" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A320B432-ECE4-4BBD-83BC-271845AE0C7D}" name="Table22" displayName="Table22" ref="B15:I22" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A320B432-ECE4-4BBD-83BC-271845AE0C7D}" name="Table22" displayName="Table22" ref="B15:I22" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="B15:I22" xr:uid="{482FB508-FA20-460E-9777-8B46DD2DCC7E}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B5AE6229-5992-428D-B083-4B4DC0EF3AF4}" name=" " dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2476DCEA-4548-4B54-AA68-8C4ECAB4D82E}" name="+, -" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{1AC0833A-D33C-48A9-A5FD-E53C886647E2}" name="*, /" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{C74CD310-58A7-4695-A22D-8509CFCB2A49}" name="(" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{03B55521-36CC-4560-854F-0207E65282CB}" name=")" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{1D82CE22-06FC-4E20-80A3-98617010C5FF}" name="i" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{4E004535-EED5-454A-A7D2-9383492DFAD3}" name="&lt;, &lt;=, &gt;, =&gt;, ==, !=" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{A6C20564-2A4C-4E85-A3CD-F925DC6793F0}" name="$" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B5AE6229-5992-428D-B083-4B4DC0EF3AF4}" name=" " dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{2476DCEA-4548-4B54-AA68-8C4ECAB4D82E}" name="+, -" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{1AC0833A-D33C-48A9-A5FD-E53C886647E2}" name="*, /" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{C74CD310-58A7-4695-A22D-8509CFCB2A49}" name="(" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{03B55521-36CC-4560-854F-0207E65282CB}" name=")" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{1D82CE22-06FC-4E20-80A3-98617010C5FF}" name="i" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{4E004535-EED5-454A-A7D2-9383492DFAD3}" name="&lt;, &lt;=, &gt;, =&gt;, ==, !=" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{A6C20564-2A4C-4E85-A3CD-F925DC6793F0}" name="$" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{57B85F91-FE8F-43C4-9E78-640B37A97736}" name="Table224" displayName="Table224" ref="B27:I34" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="B27:I34" xr:uid="{443317FB-F367-4A0E-9557-BF44F154AFE3}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{32408002-24E5-499E-8B0E-4B89EC0D4BDA}" name=" " dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{2604A20F-AED2-485F-B6DF-BC205210813F}" name="+, -" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{E57EECF3-E6D8-48F9-A5B6-E461ECEE24B2}" name="*, /" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{6117B4A4-BEF5-4FF2-949C-9B01933C66EC}" name="(" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{8528898F-87F0-4604-B729-78411940F9B7}" name=")" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{B4B08576-54CF-40B0-967D-1F0ACFD2F6E1}" name="i" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{AAA6A023-7179-4E0F-A110-749ECFB9A4B1}" name="&lt;, &lt;=, &gt;, =&gt;, ==, !=" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{A51D96B1-22F6-474E-B5C3-C90FE09D0F35}" name="$" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1138,10 +1332,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D352C2A4-EE7C-43A3-AAD2-555E1B659D04}">
-  <dimension ref="B2:AD28"/>
+  <dimension ref="B2:AD34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,10 +1346,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="24"/>
+      <c r="L2" s="26"/>
       <c r="R2" s="16"/>
       <c r="S2" s="16"/>
       <c r="T2" s="17"/>
@@ -1185,8 +1379,8 @@
       <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="26"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="28"/>
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
       <c r="T3" s="17"/>
@@ -1590,18 +1784,7 @@
         <v>5</v>
       </c>
       <c r="J17" s="17"/>
-      <c r="K17" s="18">
-        <v>13</v>
-      </c>
-      <c r="L17" t="s">
-        <v>37</v>
-      </c>
-      <c r="M17" t="s">
-        <v>39</v>
-      </c>
-      <c r="N17" t="s">
-        <v>41</v>
-      </c>
+      <c r="K17" s="18"/>
       <c r="R17" s="17"/>
       <c r="S17" s="17"/>
       <c r="T17" s="17"/>
@@ -1630,15 +1813,7 @@
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="17"/>
-      <c r="K18" s="18">
-        <v>14</v>
-      </c>
-      <c r="L18" t="s">
-        <v>38</v>
-      </c>
-      <c r="M18" t="s">
-        <v>40</v>
-      </c>
+      <c r="K18" s="18"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
@@ -1740,10 +1915,203 @@
       <c r="I23" s="17"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
       <c r="I25" s="17"/>
     </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="J28" s="17"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1752,9 +2120,10 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>